<commit_message>
processed data updated with all the workflows
</commit_message>
<xml_diff>
--- a/genome_data/processed_data/i50_10k_20k_30k_full.xlsx
+++ b/genome_data/processed_data/i50_10k_20k_30k_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\phd-support\genome_data\processed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC30ABC8-19FD-47C8-B84C-408A5B662E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2076177-0E21-4F76-A447-589CF49368F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>nodes</t>
   </si>
@@ -53,12 +53,27 @@
   <si>
     <t>Energy - 20k</t>
   </si>
+  <si>
+    <t>Watt-hr</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>30k</t>
+  </si>
+  <si>
+    <t>energy - 30k</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +204,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -535,8 +556,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -593,6 +622,2720 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>node vs enerdy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> consumption all workflows 10k,20k,30k</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>i50_10k_20k_30k_full!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>i50_10k_20k_30k_full!$L$3:$L$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>i50_10k_20k_30k_full!$M$3:$M$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.431963926316797</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70.747359803012344</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D4C7-4058-8D8B-86AD0101AEF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>i50_10k_20k_30k_full!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>i50_10k_20k_30k_full!$L$3:$L$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>i50_10k_20k_30k_full!$N$3:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>22.65935811140729</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.088381886862138</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.723218671957966</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.158611849122302</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.143194459162508</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.021207444295037</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>57.810155655784634</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63.341182973633607</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>69.706879297286108</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>75.301275820666817</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>79.136341898846268</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>83.368693287099291</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D4C7-4058-8D8B-86AD0101AEF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>i50_10k_20k_30k_full!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>30k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>i50_10k_20k_30k_full!$L$3:$L$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>i50_10k_20k_30k_full!$O$3:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>29.998505774405</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.220060521800001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.86833562853333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46.761936823477775</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.051398555038887</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.79656452022499</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.130829558999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.495840332377782</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78.370056280725009</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>82.984134920161111</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>88.422771690072224</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>95.281722621</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D4C7-4058-8D8B-86AD0101AEF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="844011103"/>
+        <c:axId val="844011519"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="844011103"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="844011519"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="844011519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Energy (Watt-hr)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="844011103"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Time vs energy consumption for</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> 30k workflow</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>i50_10k_20k_30k_full!$T$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>time - 30k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>i50_10k_20k_30k_full!$S$3:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>i50_10k_20k_30k_full!$T$3:$T$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>19013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12229</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9308</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8734</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8541</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7740</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7832</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7887</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7654</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7493</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7446</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2886-4DFD-B587-50A65683EB0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="870718079"/>
+        <c:axId val="870719327"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>i50_10k_20k_30k_full!$U$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>energy - 30k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>i50_10k_20k_30k_full!$S$3:$S$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>i50_10k_20k_30k_full!$U$3:$U$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>29.998505774405</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.220060521800001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.86833562853333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46.761936823477775</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.051398555038887</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.79656452022499</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.130829558999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.495840332377782</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78.370056280725009</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>82.984134920161111</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>88.422771690072224</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>95.281722621</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2886-4DFD-B587-50A65683EB0C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="881593327"/>
+        <c:axId val="881591663"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="870718079"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="870719327"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="870719327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="2000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Execution</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> Time</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="870718079"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1000"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="881591663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Energy (watt-hr)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="881593327"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="881593327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="881591663"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>147636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A505746-0BC8-4A27-A0E5-1123AFC341D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87EB85DA-6F0E-4650-B268-9481532EB135}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -892,10 +3635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,177 +3649,589 @@
     <col min="8" max="9" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I2" t="s">
         <v>2</v>
       </c>
+      <c r="J2" s="2"/>
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="C3" s="1"/>
+      <c r="D3" s="2">
+        <v>14924</v>
+      </c>
+      <c r="E3" s="1">
         <v>19013</v>
       </c>
-      <c r="I2">
+      <c r="H3" s="2">
+        <v>5.4659400429553902</v>
+      </c>
+      <c r="I3">
         <v>5.6800410660000002</v>
       </c>
+      <c r="J3" s="2"/>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <f>G3*C3/3600</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f>H3*D3/3600</f>
+        <v>22.65935811140729</v>
+      </c>
+      <c r="O3">
+        <f>I3*E3/3600</f>
+        <v>29.998505774405</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1">
+        <v>19013</v>
+      </c>
+      <c r="U3" s="4">
+        <v>29.998505774405</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="C4" s="1"/>
+      <c r="D4" s="2">
+        <v>10514</v>
+      </c>
+      <c r="E4" s="1">
         <v>12229</v>
       </c>
-      <c r="I3">
+      <c r="H4" s="2">
+        <v>9.6174790558021392</v>
+      </c>
+      <c r="I4">
         <v>10.36815912</v>
       </c>
+      <c r="J4" s="2"/>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <f>G4*C4/3600</f>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f>H4*D4/3600</f>
+        <v>28.088381886862138</v>
+      </c>
+      <c r="O4">
+        <f>I4*E4/3600</f>
+        <v>35.220060521800001</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="T4" s="1">
+        <v>12229</v>
+      </c>
+      <c r="U4" s="4">
+        <v>35.220060521800001</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="E4">
+      <c r="C5" s="1"/>
+      <c r="D5" s="2">
+        <v>9155</v>
+      </c>
+      <c r="E5" s="1">
         <v>10256</v>
       </c>
-      <c r="I4">
+      <c r="H5" s="2">
+        <v>13.2609052123483</v>
+      </c>
+      <c r="I5">
         <v>14.34535962</v>
       </c>
+      <c r="J5" s="2"/>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M5:O14" si="0">G5*C5/3600</f>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>33.723218671957966</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>40.86833562853333</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="T5" s="1">
+        <v>10256</v>
+      </c>
+      <c r="U5" s="4">
+        <v>40.86833562853333</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="C6" s="1"/>
+      <c r="D6" s="2">
+        <v>8548</v>
+      </c>
+      <c r="E6" s="1">
         <v>9308</v>
       </c>
-      <c r="I5">
+      <c r="H6" s="2">
+        <v>16.912845420781501</v>
+      </c>
+      <c r="I6">
         <v>18.085837189999999</v>
       </c>
+      <c r="J6" s="2"/>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>40.158611849122302</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>46.761936823477775</v>
+      </c>
+      <c r="S6">
+        <v>4</v>
+      </c>
+      <c r="T6" s="1">
+        <v>9308</v>
+      </c>
+      <c r="U6" s="4">
+        <v>46.761936823477775</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="C7" s="1"/>
+      <c r="D7" s="2">
+        <v>8123</v>
+      </c>
+      <c r="E7" s="1">
         <v>8734</v>
       </c>
-      <c r="I6">
+      <c r="H7" s="2">
+        <v>20.4500184726068</v>
+      </c>
+      <c r="I7">
         <v>21.866846209999999</v>
       </c>
+      <c r="J7" s="2"/>
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>46.143194459162508</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>53.051398555038887</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7" s="1">
+        <v>8734</v>
+      </c>
+      <c r="U7" s="4">
+        <v>53.051398555038887</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C8" s="1">
         <v>6132</v>
       </c>
-      <c r="D7">
+      <c r="D8" s="2">
         <v>7519</v>
       </c>
-      <c r="E7">
+      <c r="E8" s="1">
         <v>8541</v>
       </c>
-      <c r="G7">
-        <v>23.949770352126748</v>
-      </c>
-      <c r="H7">
-        <v>22.562799999999999</v>
-      </c>
-      <c r="I7">
+      <c r="G8">
+        <v>22.5627968256263</v>
+      </c>
+      <c r="H8" s="2">
+        <v>23.949507487626299</v>
+      </c>
+      <c r="I8">
         <v>25.204031409999999</v>
       </c>
+      <c r="J8" s="2"/>
+      <c r="L8" s="2">
+        <v>6</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>38.431963926316797</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>50.021207444295037</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>59.79656452022499</v>
+      </c>
+      <c r="S8">
+        <v>6</v>
+      </c>
+      <c r="T8" s="1">
+        <v>8541</v>
+      </c>
+      <c r="U8" s="4">
+        <v>59.79656452022499</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="E8">
+      <c r="C9" s="1"/>
+      <c r="D9" s="2">
+        <v>7542</v>
+      </c>
+      <c r="E9" s="1">
         <v>7740</v>
       </c>
-      <c r="I8">
+      <c r="H9" s="2">
+        <v>27.594346375076199</v>
+      </c>
+      <c r="I9">
         <v>28.898060260000001</v>
       </c>
+      <c r="J9" s="2"/>
+      <c r="L9">
+        <v>7</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>57.810155655784634</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>62.130829558999999</v>
+      </c>
+      <c r="S9">
+        <v>7</v>
+      </c>
+      <c r="T9" s="1">
+        <v>7740</v>
+      </c>
+      <c r="U9" s="4">
+        <v>62.130829558999999</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="E9">
+      <c r="C10" s="1"/>
+      <c r="D10" s="2">
+        <v>7347</v>
+      </c>
+      <c r="E10" s="1">
         <v>7832</v>
       </c>
-      <c r="I9">
+      <c r="H10" s="2">
+        <v>31.036921016072</v>
+      </c>
+      <c r="I10">
         <v>32.403603830000002</v>
       </c>
+      <c r="J10" s="2"/>
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>63.341182973633607</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>70.495840332377782</v>
+      </c>
+      <c r="S10">
+        <v>8</v>
+      </c>
+      <c r="T10" s="1">
+        <v>7832</v>
+      </c>
+      <c r="U10" s="4">
+        <v>70.495840332377782</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>9</v>
       </c>
-      <c r="E10">
+      <c r="C11" s="1"/>
+      <c r="D11" s="2">
+        <v>7240</v>
+      </c>
+      <c r="E11" s="1">
         <v>7887</v>
       </c>
-      <c r="I10">
+      <c r="H11" s="2">
+        <v>34.660879208595297</v>
+      </c>
+      <c r="I11">
         <v>35.771802030000003</v>
       </c>
+      <c r="J11" s="2"/>
+      <c r="L11">
+        <v>9</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>69.706879297286108</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>78.370056280725009</v>
+      </c>
+      <c r="S11">
+        <v>9</v>
+      </c>
+      <c r="T11" s="1">
+        <v>7887</v>
+      </c>
+      <c r="U11" s="4">
+        <v>78.370056280725009</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>10</v>
       </c>
-      <c r="E11">
+      <c r="C12" s="1"/>
+      <c r="D12" s="2">
+        <v>7094</v>
+      </c>
+      <c r="E12" s="1">
         <v>7654</v>
       </c>
-      <c r="I11">
+      <c r="H12" s="2">
+        <v>38.213221448322599</v>
+      </c>
+      <c r="I12">
         <v>39.030949270000001</v>
       </c>
+      <c r="J12" s="2"/>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>75.301275820666817</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>82.984134920161111</v>
+      </c>
+      <c r="S12">
+        <v>10</v>
+      </c>
+      <c r="T12" s="1">
+        <v>7654</v>
+      </c>
+      <c r="U12" s="4">
+        <v>82.984134920161111</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>11</v>
       </c>
-      <c r="E12">
+      <c r="C13" s="1"/>
+      <c r="D13" s="2">
+        <v>6853</v>
+      </c>
+      <c r="E13" s="1">
         <v>7493</v>
       </c>
-      <c r="I12">
+      <c r="H13" s="2">
+        <v>41.571695729730997</v>
+      </c>
+      <c r="I13">
         <v>42.482580820000003</v>
       </c>
+      <c r="J13" s="2"/>
+      <c r="L13">
+        <v>11</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>79.136341898846268</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>88.422771690072224</v>
+      </c>
+      <c r="S13">
+        <v>11</v>
+      </c>
+      <c r="T13" s="1">
+        <v>7493</v>
+      </c>
+      <c r="U13" s="4">
+        <v>88.422771690072224</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>12</v>
       </c>
-      <c r="C13">
+      <c r="C14" s="1">
         <v>5976</v>
       </c>
-      <c r="E13">
+      <c r="D14" s="2">
+        <v>6645</v>
+      </c>
+      <c r="E14" s="1">
         <v>7446</v>
       </c>
-      <c r="I13">
+      <c r="G14">
+        <v>42.618891447597797</v>
+      </c>
+      <c r="H14" s="2">
+        <v>45.165883496396901</v>
+      </c>
+      <c r="I14">
         <v>46.066908599999998</v>
+      </c>
+      <c r="L14">
+        <v>12</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>70.747359803012344</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>83.368693287099291</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>95.281722621</v>
+      </c>
+      <c r="S14">
+        <v>12</v>
+      </c>
+      <c r="T14" s="1">
+        <v>7446</v>
+      </c>
+      <c r="U14" s="4">
+        <v>95.281722621</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M1:O1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
important info after the meeting and new experiment
</commit_message>
<xml_diff>
--- a/genome_data/processed_data/i50_10k_20k_30k_full.xlsx
+++ b/genome_data/processed_data/i50_10k_20k_30k_full.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\phd-support\genome_data\processed_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwarade/Desktop/phd-support/genome_data/processed_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2076177-0E21-4F76-A447-589CF49368F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00717A21-FCAB-0845-9CBD-025F1072F4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="i50_10k_20k_30k_full" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>nodes</t>
   </si>
@@ -67,6 +67,60 @@
   </si>
   <si>
     <t>energy - 30k</t>
+  </si>
+  <si>
+    <t>only add energy of node when jobs are running on it.</t>
+  </si>
+  <si>
+    <t>after a certain node and time, not worthwhile to add any resources</t>
+  </si>
+  <si>
+    <t>time vs energy 10k/20k/30k</t>
+  </si>
+  <si>
+    <t>graph</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>what are nodes doing?</t>
+  </si>
+  <si>
+    <t>turn them on and off if not doing anything</t>
+  </si>
+  <si>
+    <t>number of jobs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">outcome: </t>
+  </si>
+  <si>
+    <t>better scheduler</t>
+  </si>
+  <si>
+    <t>room for improvement</t>
+  </si>
+  <si>
+    <t>above has no linear speedup</t>
+  </si>
+  <si>
+    <t>workflow does not use resources equally</t>
+  </si>
+  <si>
+    <t>&lt;- nodes are not fully being utilised and hence can be turned off.</t>
+  </si>
+  <si>
+    <t>&lt;- to max out  number of nodes have</t>
+  </si>
+  <si>
+    <t>two lines of same graph - one with energy consumption of all nodes and second with just the nodes that are working.</t>
+  </si>
+  <si>
+    <t>&lt;- dotted graph showing the nodes are ideal</t>
+  </si>
+  <si>
+    <t>&lt;- shows that if the nodes are turned off, it will be good</t>
   </si>
 </sst>
 </file>
@@ -562,10 +616,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -627,7 +681,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1381,7 +1435,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2068,6 +2122,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="881591663"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3265,16 +3320,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>147636</xdr:rowOff>
+      <xdr:rowOff>109536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3301,13 +3356,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>247649</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -3635,28 +3690,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="5" width="12" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="9" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="8" max="9" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="M1" s="3" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="M1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3701,7 +3756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3723,15 +3778,15 @@
         <v>1</v>
       </c>
       <c r="M3">
-        <f>G3*C3/3600</f>
+        <f t="shared" ref="M3:O4" si="0">G3*C3/3600</f>
         <v>0</v>
       </c>
       <c r="N3">
-        <f>H3*D3/3600</f>
+        <f t="shared" si="0"/>
         <v>22.65935811140729</v>
       </c>
       <c r="O3">
-        <f>I3*E3/3600</f>
+        <f t="shared" si="0"/>
         <v>29.998505774405</v>
       </c>
       <c r="S3">
@@ -3740,11 +3795,11 @@
       <c r="T3" s="1">
         <v>19013</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U3" s="3">
         <v>29.998505774405</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3766,15 +3821,15 @@
         <v>2</v>
       </c>
       <c r="M4">
-        <f>G4*C4/3600</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f>H4*D4/3600</f>
+        <f t="shared" si="0"/>
         <v>28.088381886862138</v>
       </c>
       <c r="O4">
-        <f>I4*E4/3600</f>
+        <f t="shared" si="0"/>
         <v>35.220060521800001</v>
       </c>
       <c r="S4">
@@ -3783,11 +3838,11 @@
       <c r="T4" s="1">
         <v>12229</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="3">
         <v>35.220060521800001</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3809,15 +3864,15 @@
         <v>3</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:O14" si="0">G5*C5/3600</f>
+        <f t="shared" ref="M5:O14" si="1">G5*C5/3600</f>
         <v>0</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33.723218671957966</v>
       </c>
       <c r="O5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40.86833562853333</v>
       </c>
       <c r="S5">
@@ -3826,11 +3881,11 @@
       <c r="T5" s="1">
         <v>10256</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5" s="3">
         <v>40.86833562853333</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3852,15 +3907,15 @@
         <v>4</v>
       </c>
       <c r="M6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40.158611849122302</v>
       </c>
       <c r="O6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46.761936823477775</v>
       </c>
       <c r="S6">
@@ -3869,11 +3924,11 @@
       <c r="T6" s="1">
         <v>9308</v>
       </c>
-      <c r="U6" s="4">
+      <c r="U6" s="3">
         <v>46.761936823477775</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3895,15 +3950,15 @@
         <v>5</v>
       </c>
       <c r="M7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46.143194459162508</v>
       </c>
       <c r="O7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53.051398555038887</v>
       </c>
       <c r="S7">
@@ -3912,11 +3967,11 @@
       <c r="T7" s="1">
         <v>8734</v>
       </c>
-      <c r="U7" s="4">
+      <c r="U7" s="3">
         <v>53.051398555038887</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3943,15 +3998,15 @@
         <v>6</v>
       </c>
       <c r="M8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38.431963926316797</v>
       </c>
       <c r="N8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50.021207444295037</v>
       </c>
       <c r="O8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59.79656452022499</v>
       </c>
       <c r="S8">
@@ -3960,11 +4015,11 @@
       <c r="T8" s="1">
         <v>8541</v>
       </c>
-      <c r="U8" s="4">
+      <c r="U8" s="3">
         <v>59.79656452022499</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3986,15 +4041,15 @@
         <v>7</v>
       </c>
       <c r="M9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57.810155655784634</v>
       </c>
       <c r="O9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62.130829558999999</v>
       </c>
       <c r="S9">
@@ -4003,11 +4058,11 @@
       <c r="T9" s="1">
         <v>7740</v>
       </c>
-      <c r="U9" s="4">
+      <c r="U9" s="3">
         <v>62.130829558999999</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4029,15 +4084,15 @@
         <v>8</v>
       </c>
       <c r="M10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.341182973633607</v>
       </c>
       <c r="O10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70.495840332377782</v>
       </c>
       <c r="S10">
@@ -4046,11 +4101,11 @@
       <c r="T10" s="1">
         <v>7832</v>
       </c>
-      <c r="U10" s="4">
+      <c r="U10" s="3">
         <v>70.495840332377782</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4072,15 +4127,15 @@
         <v>9</v>
       </c>
       <c r="M11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69.706879297286108</v>
       </c>
       <c r="O11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>78.370056280725009</v>
       </c>
       <c r="S11">
@@ -4089,11 +4144,11 @@
       <c r="T11" s="1">
         <v>7887</v>
       </c>
-      <c r="U11" s="4">
+      <c r="U11" s="3">
         <v>78.370056280725009</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4115,15 +4170,15 @@
         <v>10</v>
       </c>
       <c r="M12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>75.301275820666817</v>
       </c>
       <c r="O12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>82.984134920161111</v>
       </c>
       <c r="S12">
@@ -4132,11 +4187,11 @@
       <c r="T12" s="1">
         <v>7654</v>
       </c>
-      <c r="U12" s="4">
+      <c r="U12" s="3">
         <v>82.984134920161111</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4158,15 +4213,15 @@
         <v>11</v>
       </c>
       <c r="M13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>79.136341898846268</v>
       </c>
       <c r="O13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>88.422771690072224</v>
       </c>
       <c r="S13">
@@ -4175,11 +4230,11 @@
       <c r="T13" s="1">
         <v>7493</v>
       </c>
-      <c r="U13" s="4">
+      <c r="U13" s="3">
         <v>88.422771690072224</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4205,15 +4260,15 @@
         <v>12</v>
       </c>
       <c r="M14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70.747359803012344</v>
       </c>
       <c r="N14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>83.368693287099291</v>
       </c>
       <c r="O14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>95.281722621</v>
       </c>
       <c r="S14">
@@ -4222,8 +4277,90 @@
       <c r="T14" s="1">
         <v>7446</v>
       </c>
-      <c r="U14" s="4">
+      <c r="U14" s="3">
         <v>95.281722621</v>
+      </c>
+    </row>
+    <row r="39" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="I40" t="s">
+        <v>15</v>
+      </c>
+      <c r="L40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>14</v>
+      </c>
+      <c r="K41" t="s">
+        <v>23</v>
+      </c>
+      <c r="L41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="H42">
+        <v>2.1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" t="s">
+        <v>24</v>
+      </c>
+      <c r="L42" t="s">
+        <v>18</v>
+      </c>
+      <c r="R42" t="s">
+        <v>25</v>
+      </c>
+      <c r="X42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="H43">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K43" t="s">
+        <v>27</v>
+      </c>
+      <c r="X43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <v>3</v>
+      </c>
+      <c r="I44" t="s">
+        <v>19</v>
+      </c>
+      <c r="R44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H51" t="s">
+        <v>20</v>
+      </c>
+      <c r="I51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="I52" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jeean guy scripts, stata all graphs done
</commit_message>
<xml_diff>
--- a/genome_data/processed_data/i50_10k_20k_30k_full.xlsx
+++ b/genome_data/processed_data/i50_10k_20k_30k_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwarade/Desktop/phd-support/genome_data/processed_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A79930-6349-8349-942E-4651D6D28576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AB0A1F-9EB3-834C-9E98-3AAF92D5CCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3707,8 +3707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
new energy data computed with new script to turn the nodes off
</commit_message>
<xml_diff>
--- a/genome_data/processed_data/i50_10k_20k_30k_full.xlsx
+++ b/genome_data/processed_data/i50_10k_20k_30k_full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwarade/Desktop/phd-support/genome_data/processed_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AB0A1F-9EB3-834C-9E98-3AAF92D5CCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45E293C-DDC6-5F4E-84F6-FB83F1AF8405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>nodes</t>
   </si>
@@ -3707,8 +3707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4380,6 +4380,9 @@
       </c>
     </row>
     <row r="42" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="F42" t="s">
+        <v>34</v>
+      </c>
       <c r="G42" t="s">
         <v>31</v>
       </c>
@@ -4403,6 +4406,9 @@
       </c>
     </row>
     <row r="43" spans="4:24" x14ac:dyDescent="0.2">
+      <c r="F43" t="s">
+        <v>34</v>
+      </c>
       <c r="G43" t="s">
         <v>32</v>
       </c>

</xml_diff>